<commit_message>
fixed bug for swap scene
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel_Ini/Scene.xlsx
+++ b/_Out/NFDataCfg/Excel_Ini/Scene.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13050"/>
+    <workbookView windowWidth="21495" windowHeight="10342"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
@@ -370,10 +370,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -391,22 +391,47 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -414,53 +439,29 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -468,36 +469,14 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -505,7 +484,36 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -513,30 +521,22 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -562,7 +562,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -574,31 +622,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -616,7 +694,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -628,121 +742,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -872,75 +872,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -964,6 +895,75 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -974,148 +974,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1164,55 +1164,55 @@
     </xf>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
@@ -1541,7 +1541,6 @@
       <a:lstStyle/>
     </a:spDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
@@ -1550,24 +1549,24 @@
   <sheetPr/>
   <dimension ref="A1:P35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10:K35"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="7.45" customWidth="1"/>
-    <col min="2" max="2" width="13.7333333333333" customWidth="1"/>
-    <col min="3" max="3" width="12.7333333333333" customWidth="1"/>
-    <col min="4" max="4" width="21.45" customWidth="1"/>
-    <col min="5" max="5" width="17.0916666666667" customWidth="1"/>
-    <col min="6" max="6" width="31.95" customWidth="1"/>
+    <col min="1" max="1" width="7.45132743362832" customWidth="1"/>
+    <col min="2" max="2" width="13.7345132743363" customWidth="1"/>
+    <col min="3" max="3" width="12.7345132743363" customWidth="1"/>
+    <col min="4" max="4" width="21.4513274336283" customWidth="1"/>
+    <col min="5" max="5" width="17.0884955752212" customWidth="1"/>
+    <col min="6" max="6" width="31.9469026548673" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="8.90833333333333" customWidth="1"/>
-    <col min="9" max="11" width="27.2666666666667" customWidth="1"/>
-    <col min="12" max="12" width="9.35833333333333" customWidth="1"/>
+    <col min="8" max="8" width="8.91150442477876" customWidth="1"/>
+    <col min="9" max="11" width="27.2654867256637" customWidth="1"/>
+    <col min="12" max="12" width="9.35398230088496" customWidth="1"/>
     <col min="13" max="13" width="14" customWidth="1"/>
-    <col min="14" max="15" width="13.2666666666667" customWidth="1"/>
+    <col min="14" max="15" width="13.2654867256637" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:16">
@@ -2092,7 +2091,7 @@
         <v>1</v>
       </c>
       <c r="K11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L11">
         <v>0</v>
@@ -2139,10 +2138,10 @@
         <v>40</v>
       </c>
       <c r="J12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L12">
         <v>0</v>
@@ -2192,7 +2191,7 @@
         <v>1</v>
       </c>
       <c r="K13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L13">
         <v>0</v>
@@ -2242,7 +2241,7 @@
         <v>1</v>
       </c>
       <c r="K14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L14">
         <v>0</v>
@@ -2292,7 +2291,7 @@
         <v>1</v>
       </c>
       <c r="K15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L15">
         <v>0</v>
@@ -2342,7 +2341,7 @@
         <v>1</v>
       </c>
       <c r="K16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L16">
         <v>0</v>
@@ -2392,7 +2391,7 @@
         <v>1</v>
       </c>
       <c r="K17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L17">
         <v>0</v>
@@ -2442,7 +2441,7 @@
         <v>1</v>
       </c>
       <c r="K18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L18">
         <v>0</v>
@@ -2492,7 +2491,7 @@
         <v>1</v>
       </c>
       <c r="K19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L19">
         <v>0</v>
@@ -2542,7 +2541,7 @@
         <v>1</v>
       </c>
       <c r="K20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L20">
         <v>0</v>
@@ -2592,7 +2591,7 @@
         <v>1</v>
       </c>
       <c r="K21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L21">
         <v>0</v>
@@ -2642,7 +2641,7 @@
         <v>1</v>
       </c>
       <c r="K22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L22">
         <v>0</v>
@@ -2692,7 +2691,7 @@
         <v>1</v>
       </c>
       <c r="K23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L23">
         <v>0</v>
@@ -2742,7 +2741,7 @@
         <v>1</v>
       </c>
       <c r="K24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L24">
         <v>0</v>
@@ -2792,7 +2791,7 @@
         <v>1</v>
       </c>
       <c r="K25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L25">
         <v>0</v>
@@ -2842,7 +2841,7 @@
         <v>1</v>
       </c>
       <c r="K26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L26">
         <v>0</v>
@@ -2892,7 +2891,7 @@
         <v>1</v>
       </c>
       <c r="K27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L27">
         <v>0</v>
@@ -2942,7 +2941,7 @@
         <v>1</v>
       </c>
       <c r="K28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L28">
         <v>0</v>
@@ -2992,7 +2991,7 @@
         <v>1</v>
       </c>
       <c r="K29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L29">
         <v>0</v>
@@ -3042,7 +3041,7 @@
         <v>1</v>
       </c>
       <c r="K30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L30">
         <v>0</v>
@@ -3092,7 +3091,7 @@
         <v>1</v>
       </c>
       <c r="K31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L31">
         <v>0</v>
@@ -3142,7 +3141,7 @@
         <v>1</v>
       </c>
       <c r="K32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L32">
         <v>0</v>
@@ -3192,7 +3191,7 @@
         <v>1</v>
       </c>
       <c r="K33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L33">
         <v>0</v>
@@ -3242,7 +3241,7 @@
         <v>1</v>
       </c>
       <c r="K34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L34">
         <v>0</v>
@@ -3292,7 +3291,7 @@
         <v>1</v>
       </c>
       <c r="K35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L35">
         <v>0</v>

</xml_diff>

<commit_message>
new relive position for player
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel_Ini/Scene.xlsx
+++ b/_Out/NFDataCfg/Excel_Ini/Scene.xlsx
@@ -1,28 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27309"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/James/Desktop/NoahGameFrame/_Out/NFDataCfg/Excel_Ini/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="21495" windowHeight="10342"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27700" windowHeight="17540"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="Scene" type="4" background="1" refreshedVersion="2" saveData="1">
-    <webPr parsePre="1" consecutive="1" xl2000="1" sourceData="1" xml="1" url="D:\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Ini\NPC\Scene.xml" htmlFormat="all" htmlTables="1"/>
+  <connection id="1" name="Scene" type="4" refreshedVersion="2" background="1" saveData="1">
+    <webPr xml="1" sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="D:\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Ini\NPC\Scene.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="108">
   <si>
     <t>Id</t>
   </si>
@@ -139,9 +152,6 @@
   </si>
   <si>
     <t>../NFDataCfg/Ini/Scene/1.xml</t>
-  </si>
-  <si>
-    <t>12,4,0</t>
   </si>
   <si>
     <t>Sources/Music/Town</t>
@@ -364,18 +374,15 @@
   <si>
     <t>Guild209</t>
   </si>
+  <si>
+    <t>0,4,0</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="22">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -389,159 +396,8 @@
       <name val="宋体"/>
       <charset val="134"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="35">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -560,194 +416,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="17">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -871,251 +541,9 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1163,58 +591,16 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium7"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1541,35 +927,35 @@
       <a:lstStyle/>
     </a:spDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.45132743362832" customWidth="1"/>
-    <col min="2" max="2" width="13.7345132743363" customWidth="1"/>
-    <col min="3" max="3" width="12.7345132743363" customWidth="1"/>
-    <col min="4" max="4" width="21.4513274336283" customWidth="1"/>
-    <col min="5" max="5" width="17.0884955752212" customWidth="1"/>
-    <col min="6" max="6" width="31.9469026548673" customWidth="1"/>
+    <col min="1" max="1" width="7.5" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" customWidth="1"/>
+    <col min="6" max="6" width="32" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="8.91150442477876" customWidth="1"/>
-    <col min="9" max="11" width="27.2654867256637" customWidth="1"/>
-    <col min="12" max="12" width="9.35398230088496" customWidth="1"/>
+    <col min="8" max="8" width="8.83203125" customWidth="1"/>
+    <col min="9" max="11" width="27.33203125" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" customWidth="1"/>
     <col min="13" max="13" width="14" customWidth="1"/>
-    <col min="14" max="15" width="13.2654867256637" customWidth="1"/>
+    <col min="14" max="15" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:16">
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1619,7 +1005,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" s="2" customFormat="1" spans="1:16">
+    <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>16</v>
       </c>
@@ -1669,7 +1055,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" s="2" customFormat="1" spans="1:16">
+    <row r="3" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>19</v>
       </c>
@@ -1719,7 +1105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" s="2" customFormat="1" spans="1:16">
+    <row r="4" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
         <v>20</v>
       </c>
@@ -1769,7 +1155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" s="2" customFormat="1" spans="1:16">
+    <row r="5" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
         <v>21</v>
       </c>
@@ -1819,7 +1205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" s="2" customFormat="1" spans="1:16">
+    <row r="6" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
         <v>22</v>
       </c>
@@ -1869,7 +1255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="3" customFormat="1" spans="1:16">
+    <row r="7" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A7" s="9" t="s">
         <v>23</v>
       </c>
@@ -1919,7 +1305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" s="3" customFormat="1" spans="1:16">
+    <row r="8" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A8" s="9" t="s">
         <v>24</v>
       </c>
@@ -1969,7 +1355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" s="4" customFormat="1" ht="14.25" spans="1:16">
+    <row r="9" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A9" s="10" t="s">
         <v>25</v>
       </c>
@@ -2009,7 +1395,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A10" s="12" t="s">
         <v>36</v>
       </c>
@@ -2029,45 +1415,45 @@
         <v>38</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>39</v>
+        <v>107</v>
       </c>
       <c r="H10">
         <v>500</v>
       </c>
       <c r="I10" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="J10">
-        <v>1</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-      <c r="M10" s="13" t="s">
+      <c r="N10" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="N10" s="12" t="s">
+      <c r="O10" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="O10" s="12" t="s">
+      <c r="P10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A11" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="P10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16">
-      <c r="A11" s="12" t="s">
+      <c r="B11" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="12" t="s">
-        <v>45</v>
-      </c>
       <c r="C11" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D11">
         <v>10</v>
@@ -2076,48 +1462,48 @@
         <v>200</v>
       </c>
       <c r="F11" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" s="12" t="s">
         <v>46</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>47</v>
       </c>
       <c r="H11">
         <v>500</v>
       </c>
       <c r="I11" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="J11">
-        <v>1</v>
-      </c>
-      <c r="K11">
-        <v>1</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
-      <c r="M11" s="13" t="s">
+      <c r="N11" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="N11" s="12" t="s">
+      <c r="O11" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="O11" s="12" t="s">
-        <v>43</v>
-      </c>
       <c r="P11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A12" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" t="s">
         <v>48</v>
       </c>
-      <c r="B12" t="s">
-        <v>49</v>
-      </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D12">
         <v>10</v>
@@ -2126,48 +1512,48 @@
         <v>200</v>
       </c>
       <c r="F12" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12" s="12" t="s">
         <v>50</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>51</v>
       </c>
       <c r="H12">
         <v>500</v>
       </c>
       <c r="I12" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <v>1</v>
-      </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="M12" s="13" t="s">
-        <v>41</v>
-      </c>
       <c r="N12" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="O12" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="O12" s="12" t="s">
+      <c r="P12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A13" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="P12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16">
-      <c r="A13" s="12" t="s">
+      <c r="B13" t="s">
         <v>54</v>
       </c>
-      <c r="B13" t="s">
-        <v>55</v>
-      </c>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D13">
         <v>10</v>
@@ -2176,48 +1562,48 @@
         <v>200</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H13">
         <v>500</v>
       </c>
       <c r="I13" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="J13">
-        <v>1</v>
-      </c>
-      <c r="K13">
-        <v>1</v>
-      </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-      <c r="M13" s="13" t="s">
+      <c r="N13" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="N13" s="12" t="s">
+      <c r="O13" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="O13" s="12" t="s">
-        <v>43</v>
-      </c>
       <c r="P13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A14" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" t="s">
         <v>57</v>
       </c>
-      <c r="B14" t="s">
-        <v>58</v>
-      </c>
       <c r="C14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D14">
         <v>10</v>
@@ -2226,16 +1612,16 @@
         <v>200</v>
       </c>
       <c r="F14" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="G14" s="12" t="s">
         <v>59</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>60</v>
       </c>
       <c r="H14">
         <v>500</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J14">
         <v>1</v>
@@ -2247,27 +1633,27 @@
         <v>0</v>
       </c>
       <c r="M14" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="N14" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="N14" s="12" t="s">
+      <c r="O14" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="O14" s="12" t="s">
+      <c r="P14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A15" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="P14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16">
-      <c r="A15" s="12" t="s">
+      <c r="B15" t="s">
         <v>64</v>
       </c>
-      <c r="B15" t="s">
-        <v>65</v>
-      </c>
       <c r="C15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D15">
         <v>10</v>
@@ -2276,16 +1662,16 @@
         <v>200</v>
       </c>
       <c r="F15" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="G15" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="G15" s="12" t="s">
-        <v>67</v>
       </c>
       <c r="H15">
         <v>500</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J15">
         <v>1</v>
@@ -2297,27 +1683,27 @@
         <v>0</v>
       </c>
       <c r="M15" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N15" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="O15" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="O15" s="12" t="s">
-        <v>43</v>
-      </c>
       <c r="P15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A16" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" t="s">
         <v>68</v>
       </c>
-      <c r="B16" t="s">
-        <v>69</v>
-      </c>
       <c r="C16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D16">
         <v>10</v>
@@ -2326,16 +1712,16 @@
         <v>200</v>
       </c>
       <c r="F16" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="G16" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="G16" s="12" t="s">
-        <v>67</v>
       </c>
       <c r="H16">
         <v>500</v>
       </c>
       <c r="I16" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J16">
         <v>1</v>
@@ -2347,27 +1733,27 @@
         <v>0</v>
       </c>
       <c r="M16" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N16" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="O16" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="O16" s="12" t="s">
-        <v>43</v>
-      </c>
       <c r="P16">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A17" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" t="s">
         <v>70</v>
       </c>
-      <c r="B17" t="s">
-        <v>71</v>
-      </c>
       <c r="C17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D17">
         <v>10</v>
@@ -2376,16 +1762,16 @@
         <v>200</v>
       </c>
       <c r="F17" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="G17" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="G17" s="12" t="s">
-        <v>67</v>
       </c>
       <c r="H17">
         <v>500</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J17">
         <v>1</v>
@@ -2397,27 +1783,27 @@
         <v>0</v>
       </c>
       <c r="M17" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N17" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="O17" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="O17" s="12" t="s">
-        <v>43</v>
-      </c>
       <c r="P17">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A18" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" t="s">
         <v>72</v>
       </c>
-      <c r="B18" t="s">
-        <v>73</v>
-      </c>
       <c r="C18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D18">
         <v>10</v>
@@ -2426,16 +1812,16 @@
         <v>200</v>
       </c>
       <c r="F18" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="G18" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="G18" s="12" t="s">
-        <v>67</v>
       </c>
       <c r="H18">
         <v>500</v>
       </c>
       <c r="I18" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J18">
         <v>1</v>
@@ -2447,27 +1833,27 @@
         <v>0</v>
       </c>
       <c r="M18" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N18" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="O18" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="O18" s="12" t="s">
-        <v>43</v>
-      </c>
       <c r="P18">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A19" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" t="s">
         <v>74</v>
       </c>
-      <c r="B19" t="s">
-        <v>75</v>
-      </c>
       <c r="C19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D19">
         <v>10</v>
@@ -2476,16 +1862,16 @@
         <v>200</v>
       </c>
       <c r="F19" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="G19" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="G19" s="12" t="s">
-        <v>67</v>
       </c>
       <c r="H19">
         <v>500</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J19">
         <v>1</v>
@@ -2497,27 +1883,27 @@
         <v>0</v>
       </c>
       <c r="M19" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N19" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="O19" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="O19" s="12" t="s">
-        <v>43</v>
-      </c>
       <c r="P19">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A20" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="B20" t="s">
         <v>76</v>
       </c>
-      <c r="B20" t="s">
-        <v>77</v>
-      </c>
       <c r="C20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D20">
         <v>10</v>
@@ -2526,16 +1912,16 @@
         <v>200</v>
       </c>
       <c r="F20" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="G20" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>67</v>
       </c>
       <c r="H20">
         <v>500</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J20">
         <v>1</v>
@@ -2547,27 +1933,27 @@
         <v>0</v>
       </c>
       <c r="M20" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N20" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="O20" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="O20" s="12" t="s">
-        <v>43</v>
-      </c>
       <c r="P20">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A21" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" t="s">
         <v>78</v>
       </c>
-      <c r="B21" t="s">
-        <v>79</v>
-      </c>
       <c r="C21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D21">
         <v>10</v>
@@ -2576,16 +1962,16 @@
         <v>200</v>
       </c>
       <c r="F21" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="G21" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="G21" s="12" t="s">
-        <v>67</v>
       </c>
       <c r="H21">
         <v>500</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J21">
         <v>1</v>
@@ -2597,27 +1983,27 @@
         <v>0</v>
       </c>
       <c r="M21" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N21" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="O21" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="O21" s="12" t="s">
-        <v>43</v>
-      </c>
       <c r="P21">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A22" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B22" t="s">
         <v>80</v>
       </c>
-      <c r="B22" t="s">
-        <v>81</v>
-      </c>
       <c r="C22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D22">
         <v>10</v>
@@ -2626,16 +2012,16 @@
         <v>200</v>
       </c>
       <c r="F22" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="G22" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>67</v>
       </c>
       <c r="H22">
         <v>500</v>
       </c>
       <c r="I22" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J22">
         <v>1</v>
@@ -2647,27 +2033,27 @@
         <v>0</v>
       </c>
       <c r="M22" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N22" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="O22" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="O22" s="12" t="s">
-        <v>43</v>
-      </c>
       <c r="P22">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A23" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B23" t="s">
         <v>82</v>
       </c>
-      <c r="B23" t="s">
-        <v>83</v>
-      </c>
       <c r="C23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D23">
         <v>10</v>
@@ -2676,16 +2062,16 @@
         <v>200</v>
       </c>
       <c r="F23" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="G23" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="G23" s="12" t="s">
-        <v>67</v>
       </c>
       <c r="H23">
         <v>500</v>
       </c>
       <c r="I23" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J23">
         <v>1</v>
@@ -2697,27 +2083,27 @@
         <v>0</v>
       </c>
       <c r="M23" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N23" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="O23" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="O23" s="12" t="s">
-        <v>43</v>
-      </c>
       <c r="P23">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A24" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B24" t="s">
         <v>84</v>
       </c>
-      <c r="B24" t="s">
-        <v>85</v>
-      </c>
       <c r="C24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D24">
         <v>10</v>
@@ -2726,16 +2112,16 @@
         <v>200</v>
       </c>
       <c r="F24" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="G24" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="G24" s="12" t="s">
-        <v>67</v>
       </c>
       <c r="H24">
         <v>500</v>
       </c>
       <c r="I24" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J24">
         <v>1</v>
@@ -2747,27 +2133,27 @@
         <v>0</v>
       </c>
       <c r="M24" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N24" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="O24" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="O24" s="12" t="s">
-        <v>43</v>
-      </c>
       <c r="P24">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A25" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B25" t="s">
         <v>86</v>
       </c>
-      <c r="B25" t="s">
-        <v>87</v>
-      </c>
       <c r="C25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D25">
         <v>10</v>
@@ -2776,16 +2162,16 @@
         <v>200</v>
       </c>
       <c r="F25" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="G25" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="G25" s="12" t="s">
-        <v>67</v>
       </c>
       <c r="H25">
         <v>500</v>
       </c>
       <c r="I25" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J25">
         <v>1</v>
@@ -2797,27 +2183,27 @@
         <v>0</v>
       </c>
       <c r="M25" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N25" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="O25" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="O25" s="12" t="s">
-        <v>43</v>
-      </c>
       <c r="P25">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A26" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B26" t="s">
         <v>88</v>
       </c>
-      <c r="B26" t="s">
-        <v>89</v>
-      </c>
       <c r="C26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D26">
         <v>10</v>
@@ -2826,16 +2212,16 @@
         <v>200</v>
       </c>
       <c r="F26" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="G26" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="G26" s="12" t="s">
-        <v>67</v>
       </c>
       <c r="H26">
         <v>500</v>
       </c>
       <c r="I26" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J26">
         <v>1</v>
@@ -2847,27 +2233,27 @@
         <v>0</v>
       </c>
       <c r="M26" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N26" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="O26" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="O26" s="12" t="s">
-        <v>43</v>
-      </c>
       <c r="P26">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A27" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B27" t="s">
         <v>90</v>
       </c>
-      <c r="B27" t="s">
-        <v>91</v>
-      </c>
       <c r="C27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D27">
         <v>10</v>
@@ -2876,16 +2262,16 @@
         <v>200</v>
       </c>
       <c r="F27" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="G27" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="G27" s="12" t="s">
-        <v>67</v>
       </c>
       <c r="H27">
         <v>500</v>
       </c>
       <c r="I27" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J27">
         <v>1</v>
@@ -2897,27 +2283,27 @@
         <v>0</v>
       </c>
       <c r="M27" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N27" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="O27" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="O27" s="12" t="s">
-        <v>43</v>
-      </c>
       <c r="P27">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A28" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B28" t="s">
         <v>92</v>
       </c>
-      <c r="B28" t="s">
-        <v>93</v>
-      </c>
       <c r="C28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D28">
         <v>10</v>
@@ -2926,16 +2312,16 @@
         <v>200</v>
       </c>
       <c r="F28" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="G28" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="G28" s="12" t="s">
-        <v>67</v>
       </c>
       <c r="H28">
         <v>500</v>
       </c>
       <c r="I28" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J28">
         <v>1</v>
@@ -2947,27 +2333,27 @@
         <v>0</v>
       </c>
       <c r="M28" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N28" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="O28" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="O28" s="12" t="s">
-        <v>43</v>
-      </c>
       <c r="P28">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A29" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="B29" t="s">
         <v>94</v>
       </c>
-      <c r="B29" t="s">
-        <v>95</v>
-      </c>
       <c r="C29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D29">
         <v>10</v>
@@ -2976,16 +2362,16 @@
         <v>200</v>
       </c>
       <c r="F29" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="G29" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="G29" s="12" t="s">
-        <v>67</v>
       </c>
       <c r="H29">
         <v>500</v>
       </c>
       <c r="I29" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J29">
         <v>1</v>
@@ -2997,27 +2383,27 @@
         <v>0</v>
       </c>
       <c r="M29" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N29" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="O29" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="O29" s="12" t="s">
-        <v>43</v>
-      </c>
       <c r="P29">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A30" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="B30" t="s">
         <v>96</v>
       </c>
-      <c r="B30" t="s">
-        <v>97</v>
-      </c>
       <c r="C30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D30">
         <v>10</v>
@@ -3026,16 +2412,16 @@
         <v>200</v>
       </c>
       <c r="F30" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="G30" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="G30" s="12" t="s">
-        <v>67</v>
       </c>
       <c r="H30">
         <v>500</v>
       </c>
       <c r="I30" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J30">
         <v>1</v>
@@ -3047,27 +2433,27 @@
         <v>0</v>
       </c>
       <c r="M30" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N30" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="O30" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="O30" s="12" t="s">
-        <v>43</v>
-      </c>
       <c r="P30">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A31" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="B31" t="s">
         <v>98</v>
       </c>
-      <c r="B31" t="s">
-        <v>99</v>
-      </c>
       <c r="C31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D31">
         <v>10</v>
@@ -3076,16 +2462,16 @@
         <v>200</v>
       </c>
       <c r="F31" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="G31" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="G31" s="12" t="s">
-        <v>67</v>
       </c>
       <c r="H31">
         <v>500</v>
       </c>
       <c r="I31" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J31">
         <v>1</v>
@@ -3097,27 +2483,27 @@
         <v>0</v>
       </c>
       <c r="M31" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N31" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="O31" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="O31" s="12" t="s">
-        <v>43</v>
-      </c>
       <c r="P31">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A32" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="B32" t="s">
         <v>100</v>
       </c>
-      <c r="B32" t="s">
-        <v>101</v>
-      </c>
       <c r="C32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D32">
         <v>10</v>
@@ -3126,16 +2512,16 @@
         <v>200</v>
       </c>
       <c r="F32" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="G32" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="G32" s="12" t="s">
-        <v>67</v>
       </c>
       <c r="H32">
         <v>500</v>
       </c>
       <c r="I32" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J32">
         <v>1</v>
@@ -3147,27 +2533,27 @@
         <v>0</v>
       </c>
       <c r="M32" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N32" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="O32" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="O32" s="12" t="s">
-        <v>43</v>
-      </c>
       <c r="P32">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:16">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A33" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="B33" t="s">
         <v>102</v>
       </c>
-      <c r="B33" t="s">
-        <v>103</v>
-      </c>
       <c r="C33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D33">
         <v>10</v>
@@ -3176,16 +2562,16 @@
         <v>200</v>
       </c>
       <c r="F33" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="G33" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="G33" s="12" t="s">
-        <v>67</v>
       </c>
       <c r="H33">
         <v>500</v>
       </c>
       <c r="I33" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J33">
         <v>1</v>
@@ -3197,27 +2583,27 @@
         <v>0</v>
       </c>
       <c r="M33" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N33" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="O33" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="O33" s="12" t="s">
-        <v>43</v>
-      </c>
       <c r="P33">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:16">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A34" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B34" t="s">
         <v>104</v>
       </c>
-      <c r="B34" t="s">
-        <v>105</v>
-      </c>
       <c r="C34" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D34">
         <v>10</v>
@@ -3226,16 +2612,16 @@
         <v>200</v>
       </c>
       <c r="F34" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="G34" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="G34" s="12" t="s">
-        <v>67</v>
       </c>
       <c r="H34">
         <v>500</v>
       </c>
       <c r="I34" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J34">
         <v>1</v>
@@ -3247,27 +2633,27 @@
         <v>0</v>
       </c>
       <c r="M34" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N34" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="O34" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="O34" s="12" t="s">
-        <v>43</v>
-      </c>
       <c r="P34">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:16">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A35" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="B35" t="s">
         <v>106</v>
       </c>
-      <c r="B35" t="s">
-        <v>107</v>
-      </c>
       <c r="C35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D35">
         <v>10</v>
@@ -3276,16 +2662,16 @@
         <v>200</v>
       </c>
       <c r="F35" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="G35" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="G35" s="12" t="s">
-        <v>67</v>
       </c>
       <c r="H35">
         <v>500</v>
       </c>
       <c r="I35" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J35">
         <v>1</v>
@@ -3297,13 +2683,13 @@
         <v>0</v>
       </c>
       <c r="M35" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N35" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="O35" s="12" t="s">
         <v>42</v>
-      </c>
-      <c r="O35" s="12" t="s">
-        <v>43</v>
       </c>
       <c r="P35">
         <v>1</v>
@@ -3316,7 +2702,7 @@
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>

</xml_diff>

<commit_message>
add random home--scene-id for new player
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel_Ini/Scene.xlsx
+++ b/_Out/NFDataCfg/Excel_Ini/Scene.xlsx
@@ -1,41 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27309"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/James/Desktop/NoahGameFrame/_Out/NFDataCfg/Excel_Ini/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27700" windowHeight="17540"/>
+    <workbookView windowWidth="21495" windowHeight="10342"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="Scene" type="4" refreshedVersion="2" background="1" saveData="1">
-    <webPr xml="1" sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="D:\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Ini\NPC\Scene.xml" htmlTables="1" htmlFormat="all"/>
+  <connection id="1" name="Scene" type="4" background="1" refreshedVersion="2" saveData="1">
+    <webPr parsePre="1" consecutive="1" xl2000="1" sourceData="1" xml="1" url="D:\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Ini\NPC\Scene.xml" htmlFormat="all" htmlTables="1"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109">
   <si>
     <t>Id</t>
   </si>
@@ -64,6 +51,9 @@
     <t>SoundList</t>
   </si>
   <si>
+    <t>Tile</t>
+  </si>
+  <si>
     <t>Share</t>
   </si>
   <si>
@@ -152,6 +142,9 @@
   </si>
   <si>
     <t>../NFDataCfg/Ini/Scene/1.xml</t>
+  </si>
+  <si>
+    <t>100,114,0</t>
   </si>
   <si>
     <t>Sources/Music/Town</t>
@@ -374,15 +367,18 @@
   <si>
     <t>Guild209</t>
   </si>
-  <si>
-    <t>100,114,0</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -396,8 +392,159 @@
       <name val="宋体"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -416,8 +563,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -541,9 +874,251 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -591,16 +1166,58 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium7"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -927,35 +1544,39 @@
       <a:lstStyle/>
     </a:spDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:Q35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="F27" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10:J35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="7.5" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" customWidth="1"/>
-    <col min="4" max="4" width="21.5" customWidth="1"/>
-    <col min="5" max="5" width="17.1640625" customWidth="1"/>
+    <col min="1" max="1" width="7.50442477876106" customWidth="1"/>
+    <col min="2" max="2" width="13.6637168141593" customWidth="1"/>
+    <col min="3" max="3" width="12.6637168141593" customWidth="1"/>
+    <col min="4" max="4" width="21.5044247787611" customWidth="1"/>
+    <col min="5" max="5" width="17.1681415929204" customWidth="1"/>
     <col min="6" max="6" width="32" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="8.83203125" customWidth="1"/>
-    <col min="9" max="11" width="27.33203125" customWidth="1"/>
-    <col min="12" max="12" width="9.33203125" customWidth="1"/>
-    <col min="13" max="13" width="14" customWidth="1"/>
-    <col min="14" max="15" width="13.33203125" customWidth="1"/>
+    <col min="8" max="8" width="8.83185840707965" customWidth="1"/>
+    <col min="9" max="9" width="27.3362831858407" customWidth="1"/>
+    <col min="10" max="10" width="27.3362831858407" customWidth="1"/>
+    <col min="11" max="12" width="27.3362831858407" customWidth="1"/>
+    <col min="13" max="13" width="9.33628318584071" customWidth="1"/>
+    <col min="14" max="14" width="14" customWidth="1"/>
+    <col min="15" max="15" width="13.3362831858407" customWidth="1"/>
+    <col min="16" max="16" width="19.3185840707965" customWidth="1"/>
+    <col min="17" max="17" width="15.2743362831858" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" s="1" customFormat="1" spans="1:17">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1004,60 +1625,66 @@
       <c r="P1" s="6" t="s">
         <v>15</v>
       </c>
+      <c r="Q1" s="6" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" s="2" customFormat="1" spans="1:17">
       <c r="A2" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="G2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>17</v>
-      </c>
       <c r="H2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="8" t="s">
-        <v>17</v>
-      </c>
       <c r="J2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="O2" s="8" t="s">
         <v>18</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="O2" s="8" t="s">
-        <v>17</v>
       </c>
       <c r="P2" s="8" t="s">
         <v>18</v>
       </c>
+      <c r="Q2" s="8" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="3" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="3" s="2" customFormat="1" spans="1:17">
       <c r="A3" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B3" s="8" t="b">
         <v>0</v>
@@ -1104,10 +1731,13 @@
       <c r="P3" s="8" t="b">
         <v>0</v>
       </c>
+      <c r="Q3" s="8" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="4" s="2" customFormat="1" spans="1:17">
       <c r="A4" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" s="8" t="b">
         <v>0</v>
@@ -1154,10 +1784,13 @@
       <c r="P4" s="8" t="b">
         <v>0</v>
       </c>
+      <c r="Q4" s="8" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="5" s="2" customFormat="1" spans="1:17">
       <c r="A5" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" s="8" t="b">
         <v>0</v>
@@ -1204,10 +1837,13 @@
       <c r="P5" s="8" t="b">
         <v>0</v>
       </c>
+      <c r="Q5" s="8" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="6" s="2" customFormat="1" spans="1:17">
       <c r="A6" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B6" s="8" t="b">
         <v>0</v>
@@ -1254,10 +1890,13 @@
       <c r="P6" s="8" t="b">
         <v>0</v>
       </c>
+      <c r="Q6" s="8" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="7" s="3" customFormat="1" spans="1:17">
       <c r="A7" s="9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B7" s="3" t="b">
         <v>0</v>
@@ -1304,10 +1943,13 @@
       <c r="P7" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="Q7" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="8" s="3" customFormat="1" spans="1:17">
       <c r="A8" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" s="3" t="b">
         <v>0</v>
@@ -1354,33 +1996,36 @@
       <c r="P8" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="Q8" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="9" s="4" customFormat="1" ht="14.25" spans="1:17">
       <c r="A9" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="K9" s="11" t="s">
         <v>33</v>
@@ -1388,22 +2033,25 @@
       <c r="L9" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="M9" s="11"/>
+      <c r="M9" s="11" t="s">
+        <v>35</v>
+      </c>
       <c r="N9" s="11"/>
       <c r="O9" s="11"/>
-      <c r="P9" s="11" t="s">
-        <v>35</v>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:17">
       <c r="A10" s="12" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D10">
         <v>10</v>
@@ -1412,48 +2060,51 @@
         <v>200</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>107</v>
+        <v>40</v>
       </c>
       <c r="H10">
         <v>500</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J10">
         <v>1</v>
       </c>
       <c r="K10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L10">
         <v>0</v>
       </c>
-      <c r="M10" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="N10" s="12" t="s">
-        <v>41</v>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10" s="13" t="s">
+        <v>42</v>
       </c>
       <c r="O10" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="P10">
+        <v>43</v>
+      </c>
+      <c r="P10" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:17">
       <c r="A11" s="12" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D11">
         <v>10</v>
@@ -1462,16 +2113,16 @@
         <v>200</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H11">
         <v>500</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J11">
         <v>1</v>
@@ -1480,30 +2131,33 @@
         <v>1</v>
       </c>
       <c r="L11">
-        <v>0</v>
-      </c>
-      <c r="M11" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="N11" s="12" t="s">
-        <v>41</v>
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11" s="13" t="s">
+        <v>42</v>
       </c>
       <c r="O11" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="P11">
+        <v>43</v>
+      </c>
+      <c r="P11" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:17">
       <c r="A12" s="12" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D12">
         <v>10</v>
@@ -1512,48 +2166,51 @@
         <v>200</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H12">
         <v>500</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="M12" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="N12" s="12" t="s">
-        <v>51</v>
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12" s="13" t="s">
+        <v>42</v>
       </c>
       <c r="O12" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="P12">
+        <v>53</v>
+      </c>
+      <c r="P12" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:17">
       <c r="A13" s="12" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C13" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D13">
         <v>10</v>
@@ -1562,16 +2219,16 @@
         <v>200</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H13">
         <v>500</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J13">
         <v>1</v>
@@ -1580,30 +2237,33 @@
         <v>1</v>
       </c>
       <c r="L13">
-        <v>0</v>
-      </c>
-      <c r="M13" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="N13" s="12" t="s">
-        <v>41</v>
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13" s="13" t="s">
+        <v>42</v>
       </c>
       <c r="O13" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="P13">
+        <v>43</v>
+      </c>
+      <c r="P13" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:17">
       <c r="A14" s="12" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B14" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C14" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D14">
         <v>10</v>
@@ -1612,16 +2272,16 @@
         <v>200</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H14">
         <v>500</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J14">
         <v>1</v>
@@ -1630,30 +2290,33 @@
         <v>1</v>
       </c>
       <c r="L14">
-        <v>0</v>
-      </c>
-      <c r="M14" s="12" t="s">
-        <v>60</v>
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
       </c>
       <c r="N14" s="12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="O14" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="P14">
+        <v>63</v>
+      </c>
+      <c r="P14" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:17">
       <c r="A15" s="12" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B15" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C15" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D15">
         <v>10</v>
@@ -1662,16 +2325,16 @@
         <v>200</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H15">
         <v>500</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J15">
         <v>1</v>
@@ -1680,30 +2343,33 @@
         <v>1</v>
       </c>
       <c r="L15">
-        <v>0</v>
-      </c>
-      <c r="M15" s="12" t="s">
-        <v>60</v>
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
       </c>
       <c r="N15" s="12" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="O15" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="P15">
+        <v>43</v>
+      </c>
+      <c r="P15" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:17">
       <c r="A16" s="12" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B16" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C16" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D16">
         <v>10</v>
@@ -1712,16 +2378,16 @@
         <v>200</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H16">
         <v>500</v>
       </c>
       <c r="I16" s="12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J16">
         <v>1</v>
@@ -1730,30 +2396,33 @@
         <v>1</v>
       </c>
       <c r="L16">
-        <v>0</v>
-      </c>
-      <c r="M16" s="12" t="s">
-        <v>60</v>
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
       </c>
       <c r="N16" s="12" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="O16" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="P16">
+        <v>43</v>
+      </c>
+      <c r="P16" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q16">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:17">
       <c r="A17" s="12" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B17" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C17" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D17">
         <v>10</v>
@@ -1762,16 +2431,16 @@
         <v>200</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H17">
         <v>500</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J17">
         <v>1</v>
@@ -1780,30 +2449,33 @@
         <v>1</v>
       </c>
       <c r="L17">
-        <v>0</v>
-      </c>
-      <c r="M17" s="12" t="s">
-        <v>60</v>
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
       </c>
       <c r="N17" s="12" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="O17" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="P17">
+        <v>43</v>
+      </c>
+      <c r="P17" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q17">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:17">
       <c r="A18" s="12" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B18" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C18" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D18">
         <v>10</v>
@@ -1812,16 +2484,16 @@
         <v>200</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H18">
         <v>500</v>
       </c>
       <c r="I18" s="12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J18">
         <v>1</v>
@@ -1830,30 +2502,33 @@
         <v>1</v>
       </c>
       <c r="L18">
-        <v>0</v>
-      </c>
-      <c r="M18" s="12" t="s">
-        <v>60</v>
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
       </c>
       <c r="N18" s="12" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="O18" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="P18">
+        <v>43</v>
+      </c>
+      <c r="P18" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q18">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:17">
       <c r="A19" s="12" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B19" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C19" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D19">
         <v>10</v>
@@ -1862,16 +2537,16 @@
         <v>200</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H19">
         <v>500</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J19">
         <v>1</v>
@@ -1880,30 +2555,33 @@
         <v>1</v>
       </c>
       <c r="L19">
-        <v>0</v>
-      </c>
-      <c r="M19" s="12" t="s">
-        <v>60</v>
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
       </c>
       <c r="N19" s="12" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="O19" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="P19">
+        <v>43</v>
+      </c>
+      <c r="P19" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q19">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:17">
       <c r="A20" s="12" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B20" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C20" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D20">
         <v>10</v>
@@ -1912,16 +2590,16 @@
         <v>200</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H20">
         <v>500</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J20">
         <v>1</v>
@@ -1930,30 +2608,33 @@
         <v>1</v>
       </c>
       <c r="L20">
-        <v>0</v>
-      </c>
-      <c r="M20" s="12" t="s">
-        <v>60</v>
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
       </c>
       <c r="N20" s="12" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="O20" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="P20">
+        <v>43</v>
+      </c>
+      <c r="P20" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q20">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:17">
       <c r="A21" s="12" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B21" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C21" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D21">
         <v>10</v>
@@ -1962,16 +2643,16 @@
         <v>200</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H21">
         <v>500</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J21">
         <v>1</v>
@@ -1980,30 +2661,33 @@
         <v>1</v>
       </c>
       <c r="L21">
-        <v>0</v>
-      </c>
-      <c r="M21" s="12" t="s">
-        <v>60</v>
+        <v>1</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
       </c>
       <c r="N21" s="12" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="O21" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="P21">
+        <v>43</v>
+      </c>
+      <c r="P21" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q21">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:17">
       <c r="A22" s="12" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B22" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C22" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D22">
         <v>10</v>
@@ -2012,16 +2696,16 @@
         <v>200</v>
       </c>
       <c r="F22" s="13" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H22">
         <v>500</v>
       </c>
       <c r="I22" s="12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J22">
         <v>1</v>
@@ -2030,30 +2714,33 @@
         <v>1</v>
       </c>
       <c r="L22">
-        <v>0</v>
-      </c>
-      <c r="M22" s="12" t="s">
-        <v>60</v>
+        <v>1</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
       </c>
       <c r="N22" s="12" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="O22" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="P22">
+        <v>43</v>
+      </c>
+      <c r="P22" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q22">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:17">
       <c r="A23" s="12" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B23" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C23" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D23">
         <v>10</v>
@@ -2062,16 +2749,16 @@
         <v>200</v>
       </c>
       <c r="F23" s="13" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H23">
         <v>500</v>
       </c>
       <c r="I23" s="12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J23">
         <v>1</v>
@@ -2080,30 +2767,33 @@
         <v>1</v>
       </c>
       <c r="L23">
-        <v>0</v>
-      </c>
-      <c r="M23" s="12" t="s">
-        <v>60</v>
+        <v>1</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
       </c>
       <c r="N23" s="12" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="O23" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="P23">
+        <v>43</v>
+      </c>
+      <c r="P23" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q23">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:17">
       <c r="A24" s="12" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B24" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C24" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D24">
         <v>10</v>
@@ -2112,16 +2802,16 @@
         <v>200</v>
       </c>
       <c r="F24" s="13" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H24">
         <v>500</v>
       </c>
       <c r="I24" s="12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J24">
         <v>1</v>
@@ -2130,30 +2820,33 @@
         <v>1</v>
       </c>
       <c r="L24">
-        <v>0</v>
-      </c>
-      <c r="M24" s="12" t="s">
-        <v>60</v>
+        <v>1</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
       </c>
       <c r="N24" s="12" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="O24" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="P24">
+        <v>43</v>
+      </c>
+      <c r="P24" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q24">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:17">
       <c r="A25" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B25" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C25" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D25">
         <v>10</v>
@@ -2162,16 +2855,16 @@
         <v>200</v>
       </c>
       <c r="F25" s="13" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G25" s="12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H25">
         <v>500</v>
       </c>
       <c r="I25" s="12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J25">
         <v>1</v>
@@ -2180,30 +2873,33 @@
         <v>1</v>
       </c>
       <c r="L25">
-        <v>0</v>
-      </c>
-      <c r="M25" s="12" t="s">
-        <v>60</v>
+        <v>1</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
       </c>
       <c r="N25" s="12" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="O25" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="P25">
+        <v>43</v>
+      </c>
+      <c r="P25" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q25">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:17">
       <c r="A26" s="12" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B26" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C26" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D26">
         <v>10</v>
@@ -2212,16 +2908,16 @@
         <v>200</v>
       </c>
       <c r="F26" s="13" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G26" s="12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H26">
         <v>500</v>
       </c>
       <c r="I26" s="12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J26">
         <v>1</v>
@@ -2230,30 +2926,33 @@
         <v>1</v>
       </c>
       <c r="L26">
-        <v>0</v>
-      </c>
-      <c r="M26" s="12" t="s">
-        <v>60</v>
+        <v>1</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
       </c>
       <c r="N26" s="12" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="O26" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="P26">
+        <v>43</v>
+      </c>
+      <c r="P26" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q26">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:17">
       <c r="A27" s="12" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B27" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C27" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D27">
         <v>10</v>
@@ -2262,16 +2961,16 @@
         <v>200</v>
       </c>
       <c r="F27" s="13" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G27" s="12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H27">
         <v>500</v>
       </c>
       <c r="I27" s="12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J27">
         <v>1</v>
@@ -2280,30 +2979,33 @@
         <v>1</v>
       </c>
       <c r="L27">
-        <v>0</v>
-      </c>
-      <c r="M27" s="12" t="s">
-        <v>60</v>
+        <v>1</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
       </c>
       <c r="N27" s="12" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="O27" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="P27">
+        <v>43</v>
+      </c>
+      <c r="P27" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q27">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:17">
       <c r="A28" s="12" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B28" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C28" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D28">
         <v>10</v>
@@ -2312,16 +3014,16 @@
         <v>200</v>
       </c>
       <c r="F28" s="13" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G28" s="12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H28">
         <v>500</v>
       </c>
       <c r="I28" s="12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J28">
         <v>1</v>
@@ -2330,30 +3032,33 @@
         <v>1</v>
       </c>
       <c r="L28">
-        <v>0</v>
-      </c>
-      <c r="M28" s="12" t="s">
-        <v>60</v>
+        <v>1</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
       </c>
       <c r="N28" s="12" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="O28" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="P28">
+        <v>43</v>
+      </c>
+      <c r="P28" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q28">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:17">
       <c r="A29" s="12" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B29" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C29" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D29">
         <v>10</v>
@@ -2362,16 +3067,16 @@
         <v>200</v>
       </c>
       <c r="F29" s="13" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G29" s="12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H29">
         <v>500</v>
       </c>
       <c r="I29" s="12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J29">
         <v>1</v>
@@ -2380,30 +3085,33 @@
         <v>1</v>
       </c>
       <c r="L29">
-        <v>0</v>
-      </c>
-      <c r="M29" s="12" t="s">
-        <v>60</v>
+        <v>1</v>
+      </c>
+      <c r="M29">
+        <v>0</v>
       </c>
       <c r="N29" s="12" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="O29" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="P29">
+        <v>43</v>
+      </c>
+      <c r="P29" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q29">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:17">
       <c r="A30" s="12" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B30" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C30" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D30">
         <v>10</v>
@@ -2412,16 +3120,16 @@
         <v>200</v>
       </c>
       <c r="F30" s="13" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G30" s="12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H30">
         <v>500</v>
       </c>
       <c r="I30" s="12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J30">
         <v>1</v>
@@ -2430,30 +3138,33 @@
         <v>1</v>
       </c>
       <c r="L30">
-        <v>0</v>
-      </c>
-      <c r="M30" s="12" t="s">
-        <v>60</v>
+        <v>1</v>
+      </c>
+      <c r="M30">
+        <v>0</v>
       </c>
       <c r="N30" s="12" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="O30" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="P30">
+        <v>43</v>
+      </c>
+      <c r="P30" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q30">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:17">
       <c r="A31" s="12" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B31" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C31" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D31">
         <v>10</v>
@@ -2462,16 +3173,16 @@
         <v>200</v>
       </c>
       <c r="F31" s="13" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G31" s="12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H31">
         <v>500</v>
       </c>
       <c r="I31" s="12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J31">
         <v>1</v>
@@ -2480,30 +3191,33 @@
         <v>1</v>
       </c>
       <c r="L31">
-        <v>0</v>
-      </c>
-      <c r="M31" s="12" t="s">
-        <v>60</v>
+        <v>1</v>
+      </c>
+      <c r="M31">
+        <v>0</v>
       </c>
       <c r="N31" s="12" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="O31" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="P31">
+        <v>43</v>
+      </c>
+      <c r="P31" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q31">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:17">
       <c r="A32" s="12" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B32" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C32" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D32">
         <v>10</v>
@@ -2512,16 +3226,16 @@
         <v>200</v>
       </c>
       <c r="F32" s="13" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G32" s="12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H32">
         <v>500</v>
       </c>
       <c r="I32" s="12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J32">
         <v>1</v>
@@ -2530,30 +3244,33 @@
         <v>1</v>
       </c>
       <c r="L32">
-        <v>0</v>
-      </c>
-      <c r="M32" s="12" t="s">
-        <v>60</v>
+        <v>1</v>
+      </c>
+      <c r="M32">
+        <v>0</v>
       </c>
       <c r="N32" s="12" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="O32" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="P32">
+        <v>43</v>
+      </c>
+      <c r="P32" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q32">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:17">
       <c r="A33" s="12" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B33" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C33" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D33">
         <v>10</v>
@@ -2562,16 +3279,16 @@
         <v>200</v>
       </c>
       <c r="F33" s="13" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G33" s="12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H33">
         <v>500</v>
       </c>
       <c r="I33" s="12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J33">
         <v>1</v>
@@ -2580,30 +3297,33 @@
         <v>1</v>
       </c>
       <c r="L33">
-        <v>0</v>
-      </c>
-      <c r="M33" s="12" t="s">
-        <v>60</v>
+        <v>1</v>
+      </c>
+      <c r="M33">
+        <v>0</v>
       </c>
       <c r="N33" s="12" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="O33" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="P33">
+        <v>43</v>
+      </c>
+      <c r="P33" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q33">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:17">
       <c r="A34" s="12" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B34" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C34" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D34">
         <v>10</v>
@@ -2612,16 +3332,16 @@
         <v>200</v>
       </c>
       <c r="F34" s="13" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G34" s="12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H34">
         <v>500</v>
       </c>
       <c r="I34" s="12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J34">
         <v>1</v>
@@ -2630,30 +3350,33 @@
         <v>1</v>
       </c>
       <c r="L34">
-        <v>0</v>
-      </c>
-      <c r="M34" s="12" t="s">
-        <v>60</v>
+        <v>1</v>
+      </c>
+      <c r="M34">
+        <v>0</v>
       </c>
       <c r="N34" s="12" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="O34" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="P34">
+        <v>43</v>
+      </c>
+      <c r="P34" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q34">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:17">
       <c r="A35" s="12" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B35" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C35" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D35">
         <v>10</v>
@@ -2662,16 +3385,16 @@
         <v>200</v>
       </c>
       <c r="F35" s="13" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G35" s="12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H35">
         <v>500</v>
       </c>
       <c r="I35" s="12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J35">
         <v>1</v>
@@ -2680,29 +3403,32 @@
         <v>1</v>
       </c>
       <c r="L35">
-        <v>0</v>
-      </c>
-      <c r="M35" s="12" t="s">
-        <v>60</v>
+        <v>1</v>
+      </c>
+      <c r="M35">
+        <v>0</v>
       </c>
       <c r="N35" s="12" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="O35" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="P35">
+        <v>43</v>
+      </c>
+      <c r="P35" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q35">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A8"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:P8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J7:J8 B7:I8 K7:Q8">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A8"/>
   </dataValidations>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>

</xml_diff>

<commit_message>
set BrowseInformation option as false
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel_Ini/Scene.xlsx
+++ b/_Out/NFDataCfg/Excel_Ini/Scene.xlsx
@@ -241,10 +241,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -262,7 +262,28 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -270,6 +291,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -284,29 +313,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -315,8 +321,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -324,13 +338,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -351,38 +358,8 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -396,6 +373,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -404,9 +404,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -433,19 +433,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -457,37 +577,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -499,121 +613,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -743,17 +743,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -791,11 +785,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -845,148 +845,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1420,8 +1420,8 @@
   <sheetPr/>
   <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:B15"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1938,7 +1938,7 @@
         <v>41</v>
       </c>
       <c r="J10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K10">
         <v>1</v>

</xml_diff>

<commit_message>
it should create a new group when payer login with a single clone scene
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel_Ini/Scene.xlsx
+++ b/_Out/NFDataCfg/Excel_Ini/Scene.xlsx
@@ -243,8 +243,8 @@
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -268,8 +268,54 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -282,8 +328,69 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -298,119 +405,12 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -433,168 +433,180 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -602,18 +614,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -743,20 +743,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -780,36 +777,6 @@
         <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -840,20 +807,53 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -863,130 +863,130 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1421,7 +1421,7 @@
   <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1941,7 +1941,7 @@
         <v>0</v>
       </c>
       <c r="K10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -1994,7 +1994,7 @@
         <v>1</v>
       </c>
       <c r="K11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L11">
         <v>1</v>
@@ -2100,7 +2100,7 @@
         <v>1</v>
       </c>
       <c r="K13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L13">
         <v>1</v>
@@ -2153,7 +2153,7 @@
         <v>1</v>
       </c>
       <c r="K14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L14">
         <v>1</v>
@@ -2206,7 +2206,7 @@
         <v>1</v>
       </c>
       <c r="K15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L15">
         <v>1</v>

</xml_diff>